<commit_message>
Réalisation bouche basic + update xlsx pinout
</commit_message>
<xml_diff>
--- a/Etude/Angle_Pinout_Servo.xlsx
+++ b/Etude/Angle_Pinout_Servo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
   <si>
     <t>Pinout InMoov Quentin</t>
   </si>
@@ -341,6 +341,82 @@
   </si>
   <si>
     <t>170°(tourné vers l'exterieur)</t>
+  </si>
+  <si>
+    <t>Arduino B</t>
+  </si>
+  <si>
+    <t>Arduino Nano</t>
+  </si>
+  <si>
+    <t>Nano</t>
+  </si>
+  <si>
+    <t>Voix InMoov</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>Servo Bouche</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Néopixel Estomac (16 leds) </t>
+  </si>
+  <si>
+    <r>
+      <t>145° (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bouche ouverte</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>58° (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bouche fermé</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -400,7 +476,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="45">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -473,17 +549,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -683,15 +748,6 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -984,11 +1040,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1008,38 +1077,38 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1050,91 +1119,121 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1424,10 +1523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K25"/>
+  <dimension ref="A2:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F29" sqref="F29:F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1435,7 +1534,7 @@
     <col min="1" max="1" width="26.85546875" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" customWidth="1"/>
     <col min="7" max="7" width="23.42578125" customWidth="1"/>
@@ -1444,41 +1543,41 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E2" s="53" t="s">
+      <c r="E2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G6" s="58" t="s">
+      <c r="G6" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="H6" s="59"/>
-      <c r="I6" s="60"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="52"/>
     </row>
     <row r="7" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
@@ -1487,7 +1586,7 @@
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1496,315 +1595,374 @@
       <c r="E7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="25" t="s">
+      <c r="G7" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="26" t="s">
+      <c r="H7" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="I7" s="27" t="s">
+      <c r="I7" s="25" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="50" t="s">
+      <c r="C8" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="G8" s="37"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="39"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="37"/>
     </row>
     <row r="9" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="48"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="51"/>
+      <c r="A9" s="54"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="57"/>
       <c r="D9" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="35"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="32"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="30"/>
     </row>
     <row r="10" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="48"/>
-      <c r="B10" s="48"/>
-      <c r="C10" s="51"/>
+      <c r="A10" s="54"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="57"/>
       <c r="D10" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="35"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="32"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="30"/>
     </row>
     <row r="11" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="48"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="51"/>
+      <c r="A11" s="54"/>
+      <c r="B11" s="54"/>
+      <c r="C11" s="57"/>
       <c r="D11" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="24" t="s">
+      <c r="F11" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="35"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="32"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="30"/>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="48"/>
-      <c r="B12" s="48"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="10" t="s">
+      <c r="A12" s="54"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="30" t="s">
+      <c r="F12" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="36"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="33"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="31"/>
     </row>
     <row r="13" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="48"/>
-      <c r="B13" s="48"/>
-      <c r="C13" s="50" t="s">
+      <c r="A13" s="54"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="55"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="42"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="40"/>
     </row>
     <row r="14" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="48"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="8" t="s">
+      <c r="A14" s="54"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="56"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="32"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="30"/>
     </row>
     <row r="15" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="48"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="8" t="s">
+      <c r="A15" s="54"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="56"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="32"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="30"/>
     </row>
     <row r="16" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="48"/>
-      <c r="B16" s="48"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="8" t="s">
+      <c r="A16" s="54"/>
+      <c r="B16" s="54"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="56"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="32"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="30"/>
     </row>
     <row r="17" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="48"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="8" t="s">
+      <c r="A17" s="54"/>
+      <c r="B17" s="54"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="56"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="32"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="30"/>
     </row>
     <row r="18" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="48"/>
-      <c r="B18" s="48"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="12" t="s">
+      <c r="A18" s="54"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="56"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="33"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="31"/>
     </row>
     <row r="19" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="48"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="50" t="s">
+      <c r="A19" s="54"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="F19" s="56"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="42"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="40"/>
     </row>
     <row r="20" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="48"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="8" t="s">
+      <c r="A20" s="54"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F20" s="56"/>
-      <c r="G20" s="35" t="s">
+      <c r="F20" s="48"/>
+      <c r="G20" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="H20" s="28" t="s">
+      <c r="H20" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="I20" s="32" t="s">
+      <c r="I20" s="30" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="48"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="8" t="s">
+      <c r="A21" s="54"/>
+      <c r="B21" s="54"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="56"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="31" t="s">
+      <c r="F21" s="48"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="I21" s="45"/>
+      <c r="I21" s="43"/>
     </row>
     <row r="22" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="48"/>
-      <c r="B22" s="48"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="12" t="s">
+      <c r="A22" s="54"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E22" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="56"/>
-      <c r="G22" s="36" t="s">
+      <c r="F22" s="48"/>
+      <c r="G22" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="H22" s="44"/>
-      <c r="I22" s="46" t="s">
+      <c r="H22" s="42"/>
+      <c r="I22" s="44" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="48"/>
-      <c r="B23" s="48"/>
-      <c r="C23" s="50" t="s">
+      <c r="A23" s="54"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="21" t="s">
+      <c r="E23" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="56"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="42"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="40"/>
     </row>
     <row r="24" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="49"/>
-      <c r="B24" s="49"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="17" t="s">
+      <c r="A24" s="55"/>
+      <c r="B24" s="55"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E24" s="22" t="s">
+      <c r="E24" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="F24" s="57"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="33"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="31"/>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="B25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="53" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="53" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="E29" s="59" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" s="66"/>
+      <c r="G29" s="59"/>
+      <c r="H29" s="59"/>
+      <c r="I29" s="65"/>
+    </row>
+    <row r="30" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="54"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="64" t="s">
+        <v>67</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="67"/>
+      <c r="G30" s="70" t="s">
+        <v>71</v>
+      </c>
+      <c r="H30" s="69"/>
+      <c r="I30" s="30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="55"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="61" t="s">
+        <v>69</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="62"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="12">
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="B29:B31"/>
     <mergeCell ref="E2:K4"/>
     <mergeCell ref="F13:F24"/>
     <mergeCell ref="G6:I6"/>

</xml_diff>